<commit_message>
updates the description of CO2Captured in SysSettings.xlsx
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\Veda_models\IEMM_v60_10-1-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F10CC06-415D-43F6-A25E-2529316675F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE43A268-7379-478B-BEB1-96D10B9728E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="23040" windowHeight="11190" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4008" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="286">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -551,9 +551,6 @@
     <t>Net CO2 from electricity generation</t>
   </si>
   <si>
-    <t>CO2 Captured from electricity generation</t>
-  </si>
-  <si>
     <t>ANNUAL</t>
   </si>
   <si>
@@ -1077,6 +1074,12 @@
   </si>
   <si>
     <t>CO2 sequestered from the supply side (for accounting)</t>
+  </si>
+  <si>
+    <t>msy11_2080</t>
+  </si>
+  <si>
+    <t>CO2 Captured from electricity generation and the supply side</t>
   </si>
 </sst>
 </file>
@@ -1084,11 +1087,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="21">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
@@ -2458,135 +2461,135 @@
     <xf numFmtId="49" fontId="9" fillId="28" borderId="4">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2602,6 +2605,74 @@
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="40" fontId="44" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="40" fontId="44" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2609,82 +2680,14 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="40" fontId="44" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="40" fontId="44" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -2872,23 +2875,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
@@ -2898,13 +2901,13 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -2925,16 +2928,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="0" borderId="0">
+    <xf numFmtId="5" fontId="49" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
@@ -3870,135 +3873,135 @@
     <xf numFmtId="49" fontId="3" fillId="28" borderId="4">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4014,80 +4017,80 @@
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4964,215 +4967,215 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="58" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5278,193 +5281,193 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -9459,42 +9462,42 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15">
+    <row r="1" spans="1:1" ht="14.5">
       <c r="A1" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.5">
+      <c r="A2" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.5">
+      <c r="A3" s="14"/>
+    </row>
+    <row r="4" spans="1:1" ht="14.5">
+      <c r="A4" s="13" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
-      <c r="A2" s="14" t="s">
+    <row r="5" spans="1:1" ht="14.5">
+      <c r="A5" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15">
-      <c r="A3" s="14"/>
-    </row>
-    <row r="4" spans="1:1" ht="15">
-      <c r="A4" s="13" t="s">
+    <row r="6" spans="1:1" ht="14.5">
+      <c r="A6" s="14"/>
+    </row>
+    <row r="7" spans="1:1" ht="14.5">
+      <c r="A7" s="13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15">
-      <c r="A5" s="14" t="s">
+    <row r="8" spans="1:1" ht="14.5">
+      <c r="A8" s="14" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15">
-      <c r="A6" s="14"/>
-    </row>
-    <row r="7" spans="1:1" ht="15">
-      <c r="A7" s="13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15">
-      <c r="A8" s="14" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -9511,27 +9514,27 @@
       <selection activeCell="L38" sqref="K37:L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
         <v>123</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>124</v>
       </c>
-      <c r="J1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:10" ht="13">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -9541,12 +9544,12 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="13">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
@@ -9558,113 +9561,113 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="13">
       <c r="A5" s="12" t="s">
         <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="B8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -9684,31 +9687,31 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="13">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="13">
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="13">
       <c r="B3" s="1" t="str">
         <f>IF($A$1=2,"~TFM_UPD","~TFM_MIG")</f>
         <v>~TFM_MIG</v>
@@ -9754,7 +9757,7 @@
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9769,7 +9772,7 @@
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -9784,7 +9787,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -9798,10 +9801,10 @@
     <row r="8" spans="1:11">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -9820,13 +9823,13 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="13">
       <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" ht="13">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -9881,7 +9884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" ht="13">
       <c r="B19" s="1" t="str">
         <f>IF($A$1=2,"~TFM_INS","~TFM_INS-txt")</f>
         <v>~TFM_INS-txt</v>
@@ -9954,25 +9957,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" ht="13">
       <c r="B2" s="26" t="s">
         <v>39</v>
       </c>
@@ -9984,9 +9987,9 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" ht="13">
       <c r="B3" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>40</v>
@@ -10012,28 +10015,28 @@
     </row>
     <row r="4" spans="2:9" ht="29.25" customHeight="1" thickBot="1">
       <c r="B4" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>267</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>268</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="I4" s="18" t="s">
         <v>271</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -10123,10 +10126,10 @@
     <row r="10" spans="2:9">
       <c r="B10" s="19"/>
       <c r="C10" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>116</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>117</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>61</v>
@@ -10139,10 +10142,10 @@
     <row r="11" spans="2:9">
       <c r="B11" s="19"/>
       <c r="C11" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>61</v>
@@ -10171,10 +10174,10 @@
     <row r="13" spans="2:9">
       <c r="B13" s="19"/>
       <c r="C13" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>61</v>
@@ -10203,10 +10206,10 @@
     <row r="15" spans="2:9">
       <c r="B15" s="19"/>
       <c r="C15" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>158</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>61</v>
@@ -10317,10 +10320,10 @@
     <row r="22" spans="2:9">
       <c r="B22" s="21"/>
       <c r="C22" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>61</v>
@@ -10333,10 +10336,10 @@
     <row r="23" spans="2:9">
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>61</v>
@@ -10442,7 +10445,7 @@
         <v>92</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I29" s="21" t="s">
         <v>103</v>
@@ -10471,10 +10474,10 @@
         <v>90</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>61</v>
@@ -10487,10 +10490,10 @@
     <row r="32" spans="2:9">
       <c r="B32" s="21"/>
       <c r="C32" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>61</v>
@@ -10503,10 +10506,10 @@
     <row r="33" spans="2:11">
       <c r="B33" s="21"/>
       <c r="C33" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>61</v>
@@ -10519,10 +10522,10 @@
     <row r="34" spans="2:11">
       <c r="B34" s="21"/>
       <c r="C34" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>61</v>
@@ -10535,10 +10538,10 @@
     <row r="35" spans="2:11">
       <c r="B35" s="21"/>
       <c r="C35" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>61</v>
@@ -10551,10 +10554,10 @@
     <row r="36" spans="2:11">
       <c r="B36" s="21"/>
       <c r="C36" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>61</v>
@@ -10567,10 +10570,10 @@
     <row r="37" spans="2:11">
       <c r="B37" s="21"/>
       <c r="C37" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>61</v>
@@ -10603,14 +10606,14 @@
       <c r="C39" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="20" t="s">
-        <v>109</v>
+      <c r="D39" s="22" t="s">
+        <v>285</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>101</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
@@ -10619,16 +10622,16 @@
     <row r="40" spans="2:11">
       <c r="B40" s="21"/>
       <c r="C40" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>112</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>101</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
@@ -10637,10 +10640,10 @@
     <row r="41" spans="2:11">
       <c r="B41" s="21"/>
       <c r="C41" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>114</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>115</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>101</v>
@@ -10689,10 +10692,10 @@
         <v>98</v>
       </c>
       <c r="C44" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>159</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>160</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>61</v>
@@ -10707,10 +10710,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>199</v>
       </c>
       <c r="E45" s="21" t="s">
         <v>61</v>
@@ -10729,16 +10732,16 @@
         <v>38</v>
       </c>
       <c r="C46" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="29" t="s">
         <v>273</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>274</v>
       </c>
       <c r="E46" s="29" t="s">
         <v>61</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G46" s="28" t="s">
         <v>92</v>
@@ -10751,10 +10754,10 @@
         <v>90</v>
       </c>
       <c r="C47" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D47" s="29" t="s">
         <v>275</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>276</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>61</v>
@@ -10771,10 +10774,10 @@
         <v>90</v>
       </c>
       <c r="C48" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" s="29" t="s">
         <v>277</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>278</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>61</v>
@@ -10790,10 +10793,10 @@
         <v>98</v>
       </c>
       <c r="C49" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="D49" s="29" t="s">
         <v>279</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>280</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>101</v>
@@ -10809,10 +10812,10 @@
         <v>98</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>101</v>
@@ -10827,10 +10830,10 @@
         <v>98</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>101</v>
@@ -10856,14 +10859,14 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" ht="13">
       <c r="B2" s="26" t="s">
         <v>29</v>
       </c>
@@ -10873,12 +10876,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" ht="13">
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="13.5" thickBot="1">
@@ -10886,24 +10889,24 @@
         <v>37</v>
       </c>
       <c r="F5" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="H5" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" t="s">
         <v>204</v>
-      </c>
-      <c r="G6" t="s">
-        <v>205</v>
       </c>
       <c r="H6">
         <v>1055.55</v>
@@ -10911,13 +10914,13 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H7">
         <v>3.6</v>
@@ -10925,13 +10928,13 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" t="s">
         <v>207</v>
-      </c>
-      <c r="G8" t="s">
-        <v>208</v>
       </c>
       <c r="H8">
         <v>1000</v>
@@ -10939,13 +10942,13 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H9">
         <v>1.06</v>
@@ -10953,13 +10956,13 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H10">
         <v>0.04</v>
@@ -10967,13 +10970,13 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H11">
         <v>41.87</v>
@@ -10981,13 +10984,13 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H12">
         <v>3.5999999999999999E-3</v>
@@ -10995,13 +10998,13 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H13">
         <v>1000000</v>
@@ -11009,13 +11012,13 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G14" t="s">
         <v>219</v>
-      </c>
-      <c r="G14" t="s">
-        <v>220</v>
       </c>
       <c r="H14">
         <v>1000</v>
@@ -11023,13 +11026,13 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
+        <v>220</v>
+      </c>
+      <c r="G15" t="s">
         <v>221</v>
-      </c>
-      <c r="G15" t="s">
-        <v>222</v>
       </c>
       <c r="H15">
         <v>0.15</v>
@@ -11037,13 +11040,13 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
+        <v>222</v>
+      </c>
+      <c r="G16" t="s">
         <v>223</v>
-      </c>
-      <c r="G16" t="s">
-        <v>224</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -11051,13 +11054,13 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H17">
         <v>1000</v>
@@ -11065,13 +11068,13 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H18">
         <v>37.68</v>
@@ -11079,13 +11082,13 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H19">
         <v>2299</v>
@@ -11093,13 +11096,13 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H20">
         <v>2.78</v>
@@ -11107,13 +11110,13 @@
     </row>
     <row r="21" spans="2:8">
       <c r="B21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H21">
         <v>3.6</v>
@@ -11121,13 +11124,13 @@
     </row>
     <row r="22" spans="2:8">
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -11140,17 +11143,17 @@
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="2:8">
@@ -11165,17 +11168,17 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -11185,7 +11188,7 @@
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:2">
@@ -11195,12 +11198,12 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="2:2">
@@ -11210,52 +11213,52 @@
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -11267,33 +11270,33 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B1:H24"/>
+  <dimension ref="B1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15">
+    <row r="1" spans="2:9" ht="14.5">
       <c r="F1" s="15" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" ht="15">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="14.5">
       <c r="F2" s="15">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:9" ht="13">
       <c r="B3" s="26" t="s">
         <v>23</v>
       </c>
@@ -11301,62 +11304,66 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:9">
       <c r="B4">
         <f>MIN($F$2:$F$6)</f>
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:9" ht="13">
       <c r="B7" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:9">
       <c r="B8" t="str">
         <f>F12</f>
         <v>msy11_2050</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:9" ht="13">
       <c r="B11" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="13.5" thickBot="1">
+      <c r="B12" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="13.5" thickBot="1">
-      <c r="B12" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>227</v>
-      </c>
       <c r="F12" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>240</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
+        <v>230</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" s="10">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
+        <v>227</v>
+      </c>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" s="10">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14">
         <f>$B$4</f>
@@ -11370,13 +11377,17 @@
         <f>$B$4</f>
         <v>2017</v>
       </c>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="I14" s="27">
+        <f>$B$4</f>
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
       <c r="B15" s="10">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F15">
         <f t="shared" ref="F15:H18" si="0">F14+1</f>
@@ -11390,13 +11401,17 @@
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="I15" s="27">
+        <f t="shared" ref="I15" si="1">I14+1</f>
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
       <c r="B16" s="10">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -11410,13 +11425,17 @@
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="I16" s="27">
+        <f t="shared" ref="I16" si="2">I15+1</f>
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" s="10">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -11430,13 +11449,17 @@
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="I17" s="27">
+        <f t="shared" ref="I17" si="3">I16+1</f>
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" s="10">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -11450,13 +11473,17 @@
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="I18" s="27">
+        <f t="shared" ref="I18" si="4">I17+1</f>
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" s="10">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F19">
         <f>F17+5</f>
@@ -11469,13 +11496,17 @@
       <c r="H19">
         <v>2030</v>
       </c>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="I19" s="27">
+        <f>I17+5</f>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20" s="10">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F20">
         <f>F19+5</f>
@@ -11488,13 +11519,17 @@
       <c r="H20">
         <v>2040</v>
       </c>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="I20" s="27">
+        <f t="shared" ref="I20:I25" si="5">I19+5</f>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" s="10">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F21">
         <f>F20+5</f>
@@ -11506,13 +11541,17 @@
       <c r="H21">
         <v>2050</v>
       </c>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="I21" s="27">
+        <f t="shared" si="5"/>
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22" s="10">
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F22">
         <f>F21+5</f>
@@ -11521,23 +11560,89 @@
       <c r="G22">
         <v>2050</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="I22" s="27">
+        <f t="shared" si="5"/>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
       <c r="E23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F23">
         <f>F22+5</f>
         <v>2045</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="I23" s="27">
+        <f t="shared" si="5"/>
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
       <c r="E24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F24">
         <f>F23+5</f>
         <v>2050</v>
+      </c>
+      <c r="I24" s="27">
+        <f t="shared" si="5"/>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="E25" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="E26" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I26" s="27">
+        <f t="shared" ref="I26:I30" si="6">I25+5</f>
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="E27" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I27" s="27">
+        <f t="shared" si="6"/>
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="E28" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I28" s="27">
+        <f t="shared" si="6"/>
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="E29" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I29" s="27">
+        <f>I28+5</f>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="E30" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I30" s="27">
+        <f t="shared" si="6"/>
+        <v>2080</v>
       </c>
     </row>
   </sheetData>
@@ -11557,16 +11662,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11610,15 +11715,15 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:5" ht="13">
       <c r="C3" s="26" t="s">
         <v>12</v>
       </c>
@@ -11628,7 +11733,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>13</v>
@@ -11636,18 +11741,18 @@
     </row>
     <row r="5" spans="3:5">
       <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" t="s">
         <v>162</v>
-      </c>
-      <c r="D5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="3:5">
       <c r="C6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -11655,10 +11760,10 @@
     </row>
     <row r="7" spans="3:5">
       <c r="C7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -11666,10 +11771,10 @@
     </row>
     <row r="8" spans="3:5">
       <c r="C8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -11677,10 +11782,10 @@
     </row>
     <row r="9" spans="3:5">
       <c r="C9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -11688,10 +11793,10 @@
     </row>
     <row r="10" spans="3:5">
       <c r="C10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -11699,10 +11804,10 @@
     </row>
     <row r="11" spans="3:5">
       <c r="C11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -11710,10 +11815,10 @@
     </row>
     <row r="12" spans="3:5">
       <c r="C12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E12">
         <v>1</v>

</xml_diff>

<commit_message>
Adding a 10 year periods definition to the model
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE43A268-7379-478B-BEB1-96D10B9728E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31984F6A-F9EA-4CAF-A7EE-A8048BDF5CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4008" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="287">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1080,6 +1080,9 @@
   </si>
   <si>
     <t>CO2 Captured from electricity generation and the supply side</t>
+  </si>
+  <si>
+    <t>msy2_2080</t>
   </si>
 </sst>
 </file>
@@ -9462,40 +9465,40 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.5">
+    <row r="1" spans="1:1" ht="14.4">
       <c r="A1" s="13" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5">
+    <row r="2" spans="1:1" ht="14.4">
       <c r="A2" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5">
+    <row r="3" spans="1:1" ht="14.4">
       <c r="A3" s="14"/>
     </row>
-    <row r="4" spans="1:1" ht="14.5">
+    <row r="4" spans="1:1" ht="14.4">
       <c r="A4" s="13" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.5">
+    <row r="5" spans="1:1" ht="14.4">
       <c r="A5" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.5">
+    <row r="6" spans="1:1" ht="14.4">
       <c r="A6" s="14"/>
     </row>
-    <row r="7" spans="1:1" ht="14.5">
+    <row r="7" spans="1:1" ht="14.4">
       <c r="A7" s="13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.5">
+    <row r="8" spans="1:1" ht="14.4">
       <c r="A8" s="14" t="s">
         <v>185</v>
       </c>
@@ -9514,13 +9517,13 @@
       <selection activeCell="L38" sqref="K37:L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -9534,7 +9537,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -9544,7 +9547,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="13">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -9561,7 +9564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13">
+    <row r="5" spans="1:10">
       <c r="A5" s="12" t="s">
         <v>102</v>
       </c>
@@ -9687,31 +9690,31 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="3" width="9.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="13">
+    <row r="2" spans="1:11">
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="13">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="str">
         <f>IF($A$1=2,"~TFM_UPD","~TFM_MIG")</f>
         <v>~TFM_MIG</v>
@@ -9720,7 +9723,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1">
+    <row r="4" spans="1:11" ht="13.8" thickBot="1">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -9823,20 +9826,20 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="13">
+    <row r="11" spans="1:11">
       <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="13">
+    <row r="12" spans="1:11">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="13.5" thickBot="1">
+    <row r="13" spans="1:11" ht="13.8" thickBot="1">
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
@@ -9884,13 +9887,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="13">
+    <row r="19" spans="2:11">
       <c r="B19" s="1" t="str">
         <f>IF($A$1=2,"~TFM_INS","~TFM_INS-txt")</f>
         <v>~TFM_INS-txt</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="13.5" thickBot="1">
+    <row r="20" spans="2:11" ht="13.8" thickBot="1">
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
@@ -9957,25 +9960,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="13">
+    <row r="2" spans="2:9">
       <c r="B2" s="26" t="s">
         <v>39</v>
       </c>
@@ -9987,7 +9990,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="2:9" ht="13">
+    <row r="3" spans="2:9">
       <c r="B3" s="16" t="s">
         <v>264</v>
       </c>
@@ -10859,24 +10862,24 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="13">
+    <row r="2" spans="2:8">
       <c r="B2" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="13.5" thickBot="1">
+    <row r="3" spans="2:8" ht="13.8" thickBot="1">
       <c r="B3" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="13">
+    <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -10884,7 +10887,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="13.5" thickBot="1">
+    <row r="5" spans="2:8" ht="13.8" thickBot="1">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -11270,33 +11273,33 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="14.5">
+    <row r="1" spans="2:10" ht="14.4">
       <c r="F1" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="14.5">
+    <row r="2" spans="2:10" ht="14.4">
       <c r="F2" s="15">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="13">
+    <row r="3" spans="2:10">
       <c r="B3" s="26" t="s">
         <v>23</v>
       </c>
@@ -11304,24 +11307,24 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:10">
       <c r="B4">
         <f>MIN($F$2:$F$6)</f>
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="13">
+    <row r="7" spans="2:10">
       <c r="B7" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:10">
       <c r="B8" t="str">
         <f>F12</f>
         <v>msy11_2050</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="13">
+    <row r="11" spans="2:10">
       <c r="B11" s="26" t="s">
         <v>6</v>
       </c>
@@ -11329,7 +11332,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="13.5" thickBot="1">
+    <row r="12" spans="2:10" ht="13.8" thickBot="1">
       <c r="B12" s="25" t="s">
         <v>174</v>
       </c>
@@ -11348,8 +11351,11 @@
       <c r="I12" s="25" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="J12" s="25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
       <c r="B13" s="10">
         <v>1</v>
       </c>
@@ -11358,7 +11364,7 @@
       </c>
       <c r="I13" s="27"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:10">
       <c r="B14" s="10">
         <v>1</v>
       </c>
@@ -11381,8 +11387,11 @@
         <f>$B$4</f>
         <v>2017</v>
       </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="J14">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
       <c r="B15" s="10">
         <v>1</v>
       </c>
@@ -11405,8 +11414,11 @@
         <f t="shared" ref="I15" si="1">I14+1</f>
         <v>2018</v>
       </c>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="J15">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
       <c r="B16" s="10">
         <v>5</v>
       </c>
@@ -11429,8 +11441,11 @@
         <f t="shared" ref="I16" si="2">I15+1</f>
         <v>2019</v>
       </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="J16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="10">
         <v>5</v>
       </c>
@@ -11453,8 +11468,11 @@
         <f t="shared" ref="I17" si="3">I16+1</f>
         <v>2020</v>
       </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="J17">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="10">
         <v>5</v>
       </c>
@@ -11477,8 +11495,11 @@
         <f t="shared" ref="I18" si="4">I17+1</f>
         <v>2021</v>
       </c>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="J18">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="10">
         <v>5</v>
       </c>
@@ -11500,8 +11521,11 @@
         <f>I17+5</f>
         <v>2025</v>
       </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="J19">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="10">
         <v>5</v>
       </c>
@@ -11523,8 +11547,11 @@
         <f t="shared" ref="I20:I25" si="5">I19+5</f>
         <v>2030</v>
       </c>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="J20">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="10">
         <v>5</v>
       </c>
@@ -11545,8 +11572,11 @@
         <f t="shared" si="5"/>
         <v>2035</v>
       </c>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="J21">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="10">
         <v>5</v>
       </c>
@@ -11564,8 +11594,11 @@
         <f t="shared" si="5"/>
         <v>2040</v>
       </c>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="J22">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
       <c r="E23" t="s">
         <v>228</v>
       </c>
@@ -11577,8 +11610,11 @@
         <f t="shared" si="5"/>
         <v>2045</v>
       </c>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="J23">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
       <c r="E24" t="s">
         <v>228</v>
       </c>
@@ -11590,8 +11626,11 @@
         <f t="shared" si="5"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="25" spans="2:9">
+      <c r="J24">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="E25" s="27" t="s">
         <v>228</v>
       </c>
@@ -11600,7 +11639,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:10">
       <c r="E26" s="27" t="s">
         <v>228</v>
       </c>
@@ -11609,7 +11648,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:10">
       <c r="E27" s="27" t="s">
         <v>228</v>
       </c>
@@ -11618,7 +11657,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:10">
       <c r="E28" s="27" t="s">
         <v>228</v>
       </c>
@@ -11627,7 +11666,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:10">
       <c r="E29" s="27" t="s">
         <v>228</v>
       </c>
@@ -11636,7 +11675,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:10">
       <c r="E30" s="27" t="s">
         <v>228</v>
       </c>
@@ -11662,16 +11701,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11680,7 +11719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" thickBot="1">
+    <row r="4" spans="2:7" ht="13.8" thickBot="1">
       <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
@@ -11715,20 +11754,20 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" ht="13">
+    <row r="3" spans="3:5">
       <c r="C3" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:5" ht="13.5" thickBot="1">
+    <row r="4" spans="3:5" ht="13.8" thickBot="1">
       <c r="C4" s="25" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Deleting the commodity COALIG from the model since it has no supply-curve
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31984F6A-F9EA-4CAF-A7EE-A8048BDF5CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCA4B7-E350-4244-AC5B-C9D145629EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -99,6 +99,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>A satisfied Microsoft Office User</author>
+    <author>Mahmoud Mobir</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{61590560-D9A7-42E1-9DC4-FBCB5A0093EF}">
@@ -181,6 +182,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B64" authorId="1" shapeId="0" xr:uid="{529796A4-735E-4813-82E2-7C659793636E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahmoud Mobir:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+12-10-2021
+This commodity was deleted from the RES because there is no supply-cruve associated to it. IT drives the CO2 price like crazy when net zero emissions from ELE are modeled. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -222,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="288">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1083,6 +1109,9 @@
   </si>
   <si>
     <t>msy2_2080</t>
+  </si>
+  <si>
+    <t>Deleted from the RES</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1141,7 @@
     <numFmt numFmtId="181" formatCode="#."/>
     <numFmt numFmtId="182" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="60">
+  <fonts count="62">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1486,6 +1515,19 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="47">
@@ -9958,10 +10000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:K51"/>
+  <dimension ref="B2:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
@@ -10079,44 +10121,44 @@
     <row r="7" spans="2:9">
       <c r="B7" s="19"/>
       <c r="C7" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>61</v>
@@ -10128,11 +10170,11 @@
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="19"/>
-      <c r="C10" s="19" t="s">
-        <v>115</v>
+      <c r="C10" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>61</v>
@@ -10145,10 +10187,10 @@
     <row r="11" spans="2:9">
       <c r="B11" s="19"/>
       <c r="C11" s="21" t="s">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>61</v>
@@ -10161,10 +10203,10 @@
     <row r="12" spans="2:9">
       <c r="B12" s="19"/>
       <c r="C12" s="21" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>80</v>
+        <v>176</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>61</v>
@@ -10176,11 +10218,11 @@
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="19"/>
-      <c r="C13" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>176</v>
+      <c r="C13" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>61</v>
@@ -10192,11 +10234,11 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="19"/>
-      <c r="C14" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>81</v>
+      <c r="C14" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>61</v>
@@ -10209,10 +10251,10 @@
     <row r="15" spans="2:9">
       <c r="B15" s="19"/>
       <c r="C15" s="21" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>61</v>
@@ -10225,44 +10267,44 @@
     <row r="16" spans="2:9">
       <c r="B16" s="19"/>
       <c r="C16" s="21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="19"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="21" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
-        <v>33</v>
-      </c>
+      <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="21"/>
       <c r="C18" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>61</v>
@@ -10275,10 +10317,10 @@
     <row r="19" spans="2:9">
       <c r="B19" s="21"/>
       <c r="C19" s="21" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>61</v>
@@ -10291,10 +10333,10 @@
     <row r="20" spans="2:9">
       <c r="B20" s="21"/>
       <c r="C20" s="21" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>61</v>
@@ -10307,10 +10349,10 @@
     <row r="21" spans="2:9">
       <c r="B21" s="21"/>
       <c r="C21" s="21" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>61</v>
@@ -10323,10 +10365,10 @@
     <row r="22" spans="2:9">
       <c r="B22" s="21"/>
       <c r="C22" s="21" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>61</v>
@@ -10339,10 +10381,10 @@
     <row r="23" spans="2:9">
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>61</v>
@@ -10355,10 +10397,10 @@
     <row r="24" spans="2:9">
       <c r="B24" s="21"/>
       <c r="C24" s="21" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>61</v>
@@ -10371,10 +10413,10 @@
     <row r="25" spans="2:9">
       <c r="B25" s="21"/>
       <c r="C25" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>61</v>
@@ -10386,11 +10428,11 @@
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="21"/>
-      <c r="C26" s="21" t="s">
-        <v>66</v>
+      <c r="C26" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>61</v>
@@ -10402,11 +10444,11 @@
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="21"/>
-      <c r="C27" s="23" t="s">
-        <v>67</v>
+      <c r="C27" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>61</v>
@@ -10418,69 +10460,69 @@
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="21"/>
-      <c r="C28" s="21" t="s">
-        <v>72</v>
+      <c r="C28" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="G28" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="21"/>
       <c r="C29" s="23" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>103</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="21"/>
+      <c r="B30" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" s="23" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F30" s="21"/>
-      <c r="G30" s="21" t="s">
-        <v>33</v>
-      </c>
+      <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
     </row>
     <row r="31" spans="2:9">
-      <c r="B31" s="21" t="s">
-        <v>90</v>
-      </c>
+      <c r="B31" s="21"/>
       <c r="C31" s="23" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>61</v>
@@ -10493,10 +10535,10 @@
     <row r="32" spans="2:9">
       <c r="B32" s="21"/>
       <c r="C32" s="23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>61</v>
@@ -10509,15 +10551,15 @@
     <row r="33" spans="2:11">
       <c r="B33" s="21"/>
       <c r="C33" s="23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
@@ -10525,10 +10567,10 @@
     <row r="34" spans="2:11">
       <c r="B34" s="21"/>
       <c r="C34" s="23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>61</v>
@@ -10541,10 +10583,10 @@
     <row r="35" spans="2:11">
       <c r="B35" s="21"/>
       <c r="C35" s="23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>61</v>
@@ -10557,10 +10599,10 @@
     <row r="36" spans="2:11">
       <c r="B36" s="21"/>
       <c r="C36" s="23" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>61</v>
@@ -10571,15 +10613,17 @@
       <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" s="21"/>
+      <c r="B37" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="C37" s="23" t="s">
-        <v>192</v>
+        <v>99</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="21"/>
@@ -10587,19 +10631,19 @@
       <c r="I37" s="21"/>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="21" t="s">
-        <v>98</v>
-      </c>
+      <c r="B38" s="21"/>
       <c r="C38" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>100</v>
+        <v>106</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>285</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="21"/>
@@ -10607,10 +10651,10 @@
     <row r="39" spans="2:11">
       <c r="B39" s="21"/>
       <c r="C39" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>285</v>
+        <v>110</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>101</v>
@@ -10625,30 +10669,28 @@
     <row r="40" spans="2:11">
       <c r="B40" s="21"/>
       <c r="C40" s="23" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="21" t="s">
-        <v>112</v>
-      </c>
+      <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
     </row>
     <row r="41" spans="2:11">
       <c r="B41" s="21"/>
-      <c r="C41" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="C41" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="22" t="s">
         <v>101</v>
       </c>
       <c r="F41" s="21"/>
@@ -10657,15 +10699,17 @@
       <c r="I41" s="21"/>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" s="21"/>
-      <c r="C42" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>101</v>
+      <c r="B42" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
@@ -10674,13 +10718,13 @@
     </row>
     <row r="43" spans="2:11">
       <c r="B43" s="21" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="E43" s="21" t="s">
         <v>61</v>
@@ -10692,63 +10736,63 @@
     </row>
     <row r="44" spans="2:11">
       <c r="B44" s="21" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>61</v>
       </c>
       <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
+      <c r="I44" s="21" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="E45" s="21" t="s">
+      <c r="C45" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="E45" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21" t="s">
+      <c r="F45" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21" t="s">
-        <v>103</v>
-      </c>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
     </row>
     <row r="46" spans="2:11">
       <c r="B46" s="28" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E46" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G46" s="28" t="s">
-        <v>92</v>
-      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
     </row>
@@ -10757,10 +10801,10 @@
         <v>90</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>61</v>
@@ -10774,16 +10818,16 @@
     </row>
     <row r="48" spans="2:11" s="27" customFormat="1">
       <c r="B48" s="28" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="28"/>
@@ -10796,10 +10840,10 @@
         <v>98</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>101</v>
@@ -10815,10 +10859,10 @@
         <v>98</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>101</v>
@@ -10828,23 +10872,28 @@
       <c r="H50" s="30"/>
       <c r="I50" s="30"/>
     </row>
-    <row r="51" spans="2:10">
-      <c r="B51" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
+    <row r="64" spans="2:10">
+      <c r="B64" s="26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9">
+      <c r="B65" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11275,7 +11324,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding the commodity TOTCO2Net to the model
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCA4B7-E350-4244-AC5B-C9D145629EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20900CC-4597-4CDE-AFBD-4D8937C53186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1584" yWindow="1584" windowWidth="21492" windowHeight="12204" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="290">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1112,6 +1112,12 @@
   </si>
   <si>
     <t>Deleted from the RES</t>
+  </si>
+  <si>
+    <t>TOTCO2Net</t>
+  </si>
+  <si>
+    <t>Total Net CO2 emissions</t>
   </si>
 </sst>
 </file>
@@ -10003,7 +10009,7 @@
   <dimension ref="B2:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
@@ -10627,7 +10633,6 @@
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
       <c r="I37" s="21"/>
     </row>
     <row r="38" spans="2:11">
@@ -10871,6 +10876,24 @@
       <c r="G50" s="28"/>
       <c r="H50" s="30"/>
       <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="2:10" s="27" customFormat="1">
+      <c r="B51" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="26" t="s">

</xml_diff>

<commit_message>
Putting FX bounds on the balance of heat commodities
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20900CC-4597-4CDE-AFBD-4D8937C53186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA0B86-A4E9-4E9D-BE52-B62779A80F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="1584" windowWidth="21492" windowHeight="12204" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="290">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -10008,8 +10008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
@@ -10497,7 +10497,9 @@
       <c r="E29" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="21"/>
+      <c r="F29" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="G29" s="21" t="s">
         <v>33</v>
       </c>
@@ -10581,7 +10583,9 @@
       <c r="E34" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
@@ -10597,7 +10601,9 @@
       <c r="E35" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
@@ -10613,7 +10619,9 @@
       <c r="E36" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="23"/>
+      <c r="F36" s="24" t="s">
+        <v>112</v>
+      </c>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>

</xml_diff>

<commit_message>
adding emissions commodities to the model
  - this is done to make the net balance of the commodities defined by com_agg not affected by any FX/UP bounds on other comms
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA0B86-A4E9-4E9D-BE52-B62779A80F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE84CCD-202E-4373-9825-55DC66502488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="23040" windowHeight="12072" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="25" r:id="rId1"/>
@@ -248,7 +248,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="294">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1118,6 +1118,18 @@
   </si>
   <si>
     <t>Total Net CO2 emissions</t>
+  </si>
+  <si>
+    <t>SUPCO2-SeqAcc</t>
+  </si>
+  <si>
+    <t>ELCCO2-SeqAcc</t>
+  </si>
+  <si>
+    <t>CO2 sequestered from the supply side</t>
+  </si>
+  <si>
+    <t>CO2 sequestered from electricity generation</t>
   </si>
 </sst>
 </file>
@@ -10008,15 +10020,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="9.21875" customWidth="1"/>
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
@@ -10684,13 +10696,15 @@
       <c r="C40" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="20" t="s">
-        <v>114</v>
+      <c r="D40" s="22" t="s">
+        <v>293</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="21" t="s">
+        <v>112</v>
+      </c>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
@@ -10875,12 +10889,14 @@
         <v>281</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="28"/>
+      <c r="F50" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="G50" s="28"/>
       <c r="H50" s="30"/>
       <c r="I50" s="30"/>
@@ -10892,16 +10908,52 @@
       <c r="C51" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="28" t="s">
         <v>101</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="30"/>
       <c r="I51" s="30"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="26" t="s">

</xml_diff>